<commit_message>
Refactor dashboard: Fix DMSCO naming, enhance GL charts & resolve aggregation issues
Major refactoring addressing critical data accuracy and UI enhancements:
- Corrected all "DMASCO" references to "DMSCO" across 15 files for brand consistency
- Fixed "all quarters" aggregation logic to properly sum Q1-Q4 data instead of showing single quarters
- Enhanced GL accounts chart with color-segmented "Others" column showing individual account breakdowns
- Resolved React hooks order violations and initialization errors in Dashboard component
- Added comprehensive test coverage for aggregation fixes and validation logic

🤖 Generated with Claude Code

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haithamdata/Downloads/Mail Downloads/cost_dashboard_vis3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4A9710-8DDB-0341-BCA4-4E76151E71D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545439BD-D0BB-B84D-908F-9C41C4756936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19260" yWindow="660" windowWidth="18980" windowHeight="19860" tabRatio="709" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="160" yWindow="660" windowWidth="38080" windowHeight="23840" tabRatio="709" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q2-25 TCO " sheetId="4" r:id="rId1"/>
@@ -3062,7 +3062,7 @@
     <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3155,12 +3155,6 @@
       <b/>
       <sz val="8"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -4443,11 +4437,11 @@
   <dimension ref="A1:Z230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G85" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="Q137" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E20" sqref="E20"/>
       <selection pane="topRight" activeCell="E20" sqref="E20"/>
       <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
-      <selection pane="bottomRight" activeCell="C117" sqref="C117:C230"/>
+      <selection pane="bottomRight" activeCell="U1" sqref="U1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12581,7 +12575,7 @@
         <v>0</v>
       </c>
       <c r="Y98" s="7">
-        <f t="shared" ref="Y98:Y161" si="30">T98*P98</f>
+        <f t="shared" ref="Y98:Y116" si="30">T98*P98</f>
         <v>0</v>
       </c>
       <c r="Z98" s="26">
@@ -14129,23 +14123,23 @@
         <v>0.22</v>
       </c>
       <c r="U117" s="7">
-        <f>L117-(V117+W117+X117+Y117)</f>
+        <f t="shared" ref="U117:U148" si="32">L117-(V117+W117+X117+Y117)</f>
         <v>3359614.6745700003</v>
       </c>
       <c r="V117" s="7">
-        <f>Q117*L117</f>
+        <f t="shared" ref="V117:V153" si="33">Q117*L117</f>
         <v>259429.7046</v>
       </c>
       <c r="W117" s="7">
-        <f>R117*P117</f>
+        <f t="shared" ref="W117:W148" si="34">R117*P117</f>
         <v>0</v>
       </c>
       <c r="X117" s="17">
-        <f>S117*O117</f>
+        <f t="shared" ref="X117:X153" si="35">S117*O117</f>
         <v>657221.91832000006</v>
       </c>
       <c r="Y117" s="7">
-        <f>T117*P117</f>
+        <f t="shared" ref="Y117:Y153" si="36">T117*P117</f>
         <v>47562.112509999999</v>
       </c>
       <c r="Z117" s="15">
@@ -14209,23 +14203,23 @@
       <c r="S118" s="11"/>
       <c r="T118" s="11"/>
       <c r="U118" s="7">
-        <f>L118-(V118+W118+X118+Y118)</f>
+        <f t="shared" si="32"/>
         <v>611619.46019999997</v>
       </c>
       <c r="V118" s="7">
-        <f>Q118*L118</f>
+        <f t="shared" si="33"/>
         <v>12482.0298</v>
       </c>
       <c r="W118" s="7">
-        <f>R118*P118</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X118" s="7">
-        <f>S118*O118</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y118" s="7">
-        <f>T118*P118</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z118" s="15">
@@ -14291,23 +14285,23 @@
       </c>
       <c r="T119" s="11"/>
       <c r="U119" s="7">
-        <f>L119-(V119+W119+X119+Y119)</f>
+        <f t="shared" si="32"/>
         <v>2119348.3453100002</v>
       </c>
       <c r="V119" s="7">
-        <f>Q119*L119</f>
+        <f t="shared" si="33"/>
         <v>112611.49550000002</v>
       </c>
       <c r="W119" s="7">
-        <f>R119*P119</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X119" s="17">
-        <f>S119*O119</f>
+        <f t="shared" si="35"/>
         <v>20270.069190000002</v>
       </c>
       <c r="Y119" s="7">
-        <f>T119*P119</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z119" s="15">
@@ -14369,23 +14363,23 @@
       <c r="S120" s="11"/>
       <c r="T120" s="11"/>
       <c r="U120" s="7">
-        <f>L120-(V120+W120+X120+Y120)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V120" s="7">
-        <f>Q120*L120</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="W120" s="7">
-        <f>R120*P120</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X120" s="7">
-        <f>S120*O120</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y120" s="7">
-        <f>T120*P120</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z120" s="15">
@@ -14453,23 +14447,23 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="U121" s="7">
-        <f>L121-(V121+W121+X121+Y121)</f>
+        <f t="shared" si="32"/>
         <v>930141.98269500001</v>
       </c>
       <c r="V121" s="7">
-        <f>Q121*L121</f>
+        <f t="shared" si="33"/>
         <v>92259.349050000004</v>
       </c>
       <c r="W121" s="7">
-        <f>R121*P121</f>
+        <f t="shared" si="34"/>
         <v>185357.419455</v>
       </c>
       <c r="X121" s="7">
-        <f>S121*O121</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y121" s="7">
-        <f>T121*P121</f>
+        <f t="shared" si="36"/>
         <v>469683.95880000002</v>
       </c>
       <c r="Z121" s="15">
@@ -14535,23 +14529,23 @@
       <c r="S122" s="11"/>
       <c r="T122" s="11"/>
       <c r="U122" s="7">
-        <f>L122-(V122+W122+X122+Y122)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V122" s="7">
-        <f>Q122*L122</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="W122" s="7">
-        <f>R122*P122</f>
+        <f t="shared" si="34"/>
         <v>1000816.33</v>
       </c>
       <c r="X122" s="7">
-        <f>S122*O122</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y122" s="7">
-        <f>T122*P122</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z122" s="15">
@@ -14619,23 +14613,23 @@
         <v>0.22</v>
       </c>
       <c r="U123" s="7">
-        <f>L123-(V123+W123+X123+Y123)</f>
+        <f t="shared" si="32"/>
         <v>544370.6002799999</v>
       </c>
       <c r="V123" s="7">
-        <f>Q123*L123</f>
+        <f t="shared" si="33"/>
         <v>35533.328999999998</v>
       </c>
       <c r="W123" s="7">
-        <f>R123*P123</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X123" s="17">
-        <f>S123*O123</f>
+        <f t="shared" si="35"/>
         <v>115127.98596000001</v>
       </c>
       <c r="Y123" s="7">
-        <f>T123*P123</f>
+        <f t="shared" si="36"/>
         <v>15634.66476</v>
       </c>
       <c r="Z123" s="15">
@@ -14699,23 +14693,23 @@
       </c>
       <c r="T124" s="11"/>
       <c r="U124" s="7">
-        <f>L124-(V124+W124+X124+Y124)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V124" s="7">
-        <f>Q124*L124</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="W124" s="7">
-        <f>R124*P124</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X124" s="7">
-        <f>S124*O124</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y124" s="7">
-        <f>T124*P124</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z124" s="15">
@@ -14781,23 +14775,23 @@
         <v>0.25</v>
       </c>
       <c r="U125" s="7">
-        <f>L125-(V125+W125+X125+Y125)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V125" s="7">
-        <f>Q125*L125</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="W125" s="7">
-        <f>R125*P125</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X125" s="7">
-        <f>S125*O125</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y125" s="7">
-        <f>T125*P125</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z125" s="15">
@@ -14865,23 +14859,23 @@
         <v>0.18</v>
       </c>
       <c r="U126" s="7">
-        <f>L126-(V126+W126+X126+Y126)</f>
+        <f t="shared" si="32"/>
         <v>99794.442720000006</v>
       </c>
       <c r="V126" s="7">
-        <f>Q126*L126</f>
+        <f t="shared" si="33"/>
         <v>7637.3297999999995</v>
       </c>
       <c r="W126" s="7">
-        <f>R126*P126</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X126" s="7">
-        <f>S126*O126</f>
+        <f t="shared" si="35"/>
         <v>15274.659600000001</v>
       </c>
       <c r="Y126" s="7">
-        <f>T126*P126</f>
+        <f t="shared" si="36"/>
         <v>4582.3978800000004</v>
       </c>
       <c r="Z126" s="26">
@@ -14947,23 +14941,23 @@
         <v>0.25</v>
       </c>
       <c r="U127" s="7">
-        <f>L127-(V127+W127+X127+Y127)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V127" s="7">
-        <f>Q127*L127</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="W127" s="7">
-        <f>R127*P127</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X127" s="7">
-        <f>S127*O127</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y127" s="7">
-        <f>T127*P127</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z127" s="26">
@@ -15031,23 +15025,23 @@
         <v>0.1</v>
       </c>
       <c r="U128" s="7">
-        <f>L128-(V128+W128+X128+Y128)</f>
+        <f t="shared" si="32"/>
         <v>73994.869200000001</v>
       </c>
       <c r="V128" s="7">
-        <f>Q128*L128</f>
+        <f t="shared" si="33"/>
         <v>5285.3478000000005</v>
       </c>
       <c r="W128" s="7">
-        <f>R128*P128</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X128" s="7">
-        <f>S128*O128</f>
+        <f t="shared" si="35"/>
         <v>7928.0217000000011</v>
       </c>
       <c r="Y128" s="7">
-        <f>T128*P128</f>
+        <f t="shared" si="36"/>
         <v>880.89130000000011</v>
       </c>
       <c r="Z128" s="26">
@@ -15113,23 +15107,23 @@
         <v>0.25</v>
       </c>
       <c r="U129" s="7">
-        <f>L129-(V129+W129+X129+Y129)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V129" s="7">
-        <f>Q129*L129</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="W129" s="7">
-        <f>R129*P129</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X129" s="7">
-        <f>S129*O129</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y129" s="7">
-        <f>T129*P129</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z129" s="26">
@@ -15197,23 +15191,23 @@
         <v>0.18</v>
       </c>
       <c r="U130" s="7">
-        <f>L130-(V130+W130+X130+Y130)</f>
+        <f t="shared" si="32"/>
         <v>1434750.9856799999</v>
       </c>
       <c r="V130" s="7">
-        <f>Q130*L130</f>
+        <f t="shared" si="33"/>
         <v>97061.874800000005</v>
       </c>
       <c r="W130" s="7">
-        <f>R130*P130</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X130" s="7">
-        <f>S130*O130</f>
+        <f t="shared" si="35"/>
         <v>169417.09056000001</v>
       </c>
       <c r="Y130" s="7">
-        <f>T130*P130</f>
+        <f t="shared" si="36"/>
         <v>63531.408960000008</v>
       </c>
       <c r="Z130" s="15">
@@ -15279,23 +15273,23 @@
         <v>0.25</v>
       </c>
       <c r="U131" s="7">
-        <f>L131-(V131+W131+X131+Y131)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V131" s="7">
-        <f>Q131*L131</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="W131" s="7">
-        <f>R131*P131</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X131" s="7">
-        <f>S131*O131</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y131" s="7">
-        <f>T131*P131</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z131" s="26">
@@ -15361,23 +15355,23 @@
         <v>0.25</v>
       </c>
       <c r="U132" s="7">
-        <f>L132-(V132+W132+X132+Y132)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V132" s="7">
-        <f>Q132*L132</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="W132" s="7">
-        <f>R132*P132</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X132" s="7">
-        <f>S132*O132</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y132" s="7">
-        <f>T132*P132</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z132" s="26">
@@ -15445,23 +15439,23 @@
         <v>0.25</v>
       </c>
       <c r="U133" s="7">
-        <f>L133-(V133+W133+X133+Y133)</f>
+        <f t="shared" si="32"/>
         <v>67408.2</v>
       </c>
       <c r="V133" s="7">
-        <f>Q133*L133</f>
+        <f t="shared" si="33"/>
         <v>4993.2</v>
       </c>
       <c r="W133" s="7">
-        <f>R133*P133</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X133" s="7">
-        <f>S133*O133</f>
+        <f t="shared" si="35"/>
         <v>6657.6</v>
       </c>
       <c r="Y133" s="7">
-        <f>T133*P133</f>
+        <f t="shared" si="36"/>
         <v>4161</v>
       </c>
       <c r="Z133" s="26">
@@ -15529,23 +15523,23 @@
         <v>0.1</v>
       </c>
       <c r="U134" s="7">
-        <f>L134-(V134+W134+X134+Y134)</f>
+        <f t="shared" si="32"/>
         <v>763283.15162999998</v>
       </c>
       <c r="V134" s="7">
-        <f>Q134*L134</f>
+        <f t="shared" si="33"/>
         <v>53942.272199999999</v>
       </c>
       <c r="W134" s="7">
-        <f>R134*P134</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X134" s="7">
-        <f>S134*O134</f>
+        <f t="shared" si="35"/>
         <v>72822.067469999995</v>
       </c>
       <c r="Y134" s="7">
-        <f>T134*P134</f>
+        <f t="shared" si="36"/>
         <v>8990.3787000000011</v>
       </c>
       <c r="Z134" s="15">
@@ -15613,23 +15607,23 @@
         <v>0.25</v>
       </c>
       <c r="U135" s="7">
-        <f>L135-(V135+W135+X135+Y135)</f>
+        <f t="shared" si="32"/>
         <v>6008.3585999999996</v>
       </c>
       <c r="V135" s="7">
-        <f>Q135*L135</f>
+        <f t="shared" si="33"/>
         <v>459.23759999999999</v>
       </c>
       <c r="W135" s="7">
-        <f>R135*P135</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X135" s="7">
-        <f>S135*O135</f>
+        <f t="shared" si="35"/>
         <v>1090.6893</v>
       </c>
       <c r="Y135" s="7">
-        <f>T135*P135</f>
+        <f t="shared" si="36"/>
         <v>95.674500000000009</v>
       </c>
       <c r="Z135" s="15">
@@ -15697,23 +15691,23 @@
         <v>0.25</v>
       </c>
       <c r="U136" s="7">
-        <f>L136-(V136+W136+X136+Y136)</f>
+        <f t="shared" si="32"/>
         <v>41648.868000000002</v>
       </c>
       <c r="V136" s="7">
-        <f>Q136*L136</f>
+        <f t="shared" si="33"/>
         <v>2960.8199999999997</v>
       </c>
       <c r="W136" s="7">
-        <f>R136*P136</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X136" s="7">
-        <f>S136*O136</f>
+        <f t="shared" si="35"/>
         <v>1036.2869999999998</v>
       </c>
       <c r="Y136" s="7">
-        <f>T136*P136</f>
+        <f t="shared" si="36"/>
         <v>3701.0249999999996</v>
       </c>
       <c r="Z136" s="15">
@@ -15781,23 +15775,23 @@
         <v>0.25</v>
       </c>
       <c r="U137" s="7">
-        <f>L137-(V137+W137+X137+Y137)</f>
+        <f t="shared" si="32"/>
         <v>59325.443639999998</v>
       </c>
       <c r="V137" s="7">
-        <f>Q137*L137</f>
+        <f t="shared" si="33"/>
         <v>4217.4485999999997</v>
       </c>
       <c r="W137" s="7">
-        <f>R137*P137</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X137" s="7">
-        <f>S137*O137</f>
+        <f t="shared" si="35"/>
         <v>1476.1070099999997</v>
       </c>
       <c r="Y137" s="7">
-        <f>T137*P137</f>
+        <f t="shared" si="36"/>
         <v>5271.8107499999996</v>
       </c>
       <c r="Z137" s="15">
@@ -15865,23 +15859,23 @@
         <v>0.25</v>
       </c>
       <c r="U138" s="7">
-        <f>L138-(V138+W138+X138+Y138)</f>
+        <f t="shared" si="32"/>
         <v>24209.253799999999</v>
       </c>
       <c r="V138" s="7">
-        <f>Q138*L138</f>
+        <f t="shared" si="33"/>
         <v>1721.037</v>
       </c>
       <c r="W138" s="7">
-        <f>R138*P138</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X138" s="7">
-        <f>S138*O138</f>
+        <f t="shared" si="35"/>
         <v>602.36294999999996</v>
       </c>
       <c r="Y138" s="7">
-        <f>T138*P138</f>
+        <f t="shared" si="36"/>
         <v>2151.2962499999999</v>
       </c>
       <c r="Z138" s="15">
@@ -15949,23 +15943,23 @@
         <v>0.25</v>
       </c>
       <c r="U139" s="7">
-        <f>L139-(V139+W139+X139+Y139)</f>
+        <f t="shared" si="32"/>
         <v>397.5</v>
       </c>
       <c r="V139" s="7">
-        <f>Q139*L139</f>
+        <f t="shared" si="33"/>
         <v>30</v>
       </c>
       <c r="W139" s="7">
-        <f>R139*P139</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X139" s="7">
-        <f>S139*O139</f>
+        <f t="shared" si="35"/>
         <v>35</v>
       </c>
       <c r="Y139" s="7">
-        <f>T139*P139</f>
+        <f t="shared" si="36"/>
         <v>37.5</v>
       </c>
       <c r="Z139" s="15">
@@ -16033,23 +16027,23 @@
         <v>0.25</v>
       </c>
       <c r="U140" s="7">
-        <f>L140-(V140+W140+X140+Y140)</f>
+        <f t="shared" si="32"/>
         <v>536.625</v>
       </c>
       <c r="V140" s="7">
-        <f>Q140*L140</f>
+        <f t="shared" si="33"/>
         <v>40.5</v>
       </c>
       <c r="W140" s="7">
-        <f>R140*P140</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X140" s="7">
-        <f>S140*O140</f>
+        <f t="shared" si="35"/>
         <v>47.25</v>
       </c>
       <c r="Y140" s="7">
-        <f>T140*P140</f>
+        <f t="shared" si="36"/>
         <v>50.625</v>
       </c>
       <c r="Z140" s="15">
@@ -16115,23 +16109,23 @@
         <v>0.25</v>
       </c>
       <c r="U141" s="7">
-        <f>L141-(V141+W141+X141+Y141)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="V141" s="7">
-        <f>Q141*L141</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="W141" s="7">
-        <f>R141*P141</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X141" s="7">
-        <f>S141*O141</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y141" s="7">
-        <f>T141*P141</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z141" s="15">
@@ -16199,23 +16193,23 @@
         <v>0.25</v>
       </c>
       <c r="U142" s="7">
-        <f>L142-(V142+W142+X142+Y142)</f>
+        <f t="shared" si="32"/>
         <v>59924.715000000004</v>
       </c>
       <c r="V142" s="7">
-        <f>Q142*L142</f>
+        <f t="shared" si="33"/>
         <v>4522.62</v>
       </c>
       <c r="W142" s="7">
-        <f>R142*P142</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X142" s="7">
-        <f>S142*O142</f>
+        <f t="shared" si="35"/>
         <v>5276.3899999999994</v>
       </c>
       <c r="Y142" s="7">
-        <f>T142*P142</f>
+        <f t="shared" si="36"/>
         <v>5653.2749999999996</v>
       </c>
       <c r="Z142" s="15">
@@ -16283,23 +16277,23 @@
         <v>0.18</v>
       </c>
       <c r="U143" s="7">
-        <f>L143-(V143+W143+X143+Y143)</f>
+        <f t="shared" si="32"/>
         <v>541139.65360000008</v>
       </c>
       <c r="V143" s="7">
-        <f>Q143*L143</f>
+        <f t="shared" si="33"/>
         <v>41413.749000000003</v>
       </c>
       <c r="W143" s="7">
-        <f>R143*P143</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X143" s="17">
-        <f>S143*O143</f>
+        <f t="shared" si="35"/>
         <v>82827.498000000007</v>
       </c>
       <c r="Y143" s="7">
-        <f>T143*P143</f>
+        <f t="shared" si="36"/>
         <v>24848.249400000001</v>
       </c>
       <c r="Z143" s="15">
@@ -16367,23 +16361,23 @@
         <v>0.19</v>
       </c>
       <c r="U144" s="7">
-        <f>L144-(V144+W144+X144+Y144)</f>
+        <f t="shared" si="32"/>
         <v>364531.38749999995</v>
       </c>
       <c r="V144" s="7">
-        <f>Q144*L144</f>
+        <f t="shared" si="33"/>
         <v>29162.510999999999</v>
       </c>
       <c r="W144" s="7">
-        <f>R144*P144</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="X144" s="7">
-        <f>S144*O144</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y144" s="7">
-        <f>T144*P144</f>
+        <f t="shared" si="36"/>
         <v>92347.951499999996</v>
       </c>
       <c r="Z144" s="15">
@@ -16453,23 +16447,23 @@
         <v>0.15</v>
       </c>
       <c r="U145" s="7">
-        <f>L145-(V145+W145+X145+Y145)</f>
+        <f t="shared" si="32"/>
         <v>6110125.7910350002</v>
       </c>
       <c r="V145" s="7">
-        <f>Q145*L145</f>
+        <f t="shared" si="33"/>
         <v>461431.77779999998</v>
       </c>
       <c r="W145" s="7">
-        <f>R145*P145</f>
+        <f t="shared" si="34"/>
         <v>99976.885190000001</v>
       </c>
       <c r="X145" s="7">
-        <f>S145*O145</f>
+        <f t="shared" si="35"/>
         <v>269168.53704999998</v>
       </c>
       <c r="Y145" s="7">
-        <f>T145*P145</f>
+        <f t="shared" si="36"/>
         <v>749826.63892499998</v>
       </c>
       <c r="Z145" s="15">
@@ -16539,23 +16533,23 @@
         <v>0.06</v>
       </c>
       <c r="U146" s="7">
-        <f>L146-(V146+W146+X146+Y146)</f>
+        <f t="shared" si="32"/>
         <v>4156083.6570750005</v>
       </c>
       <c r="V146" s="7">
-        <f>Q146*L146</f>
+        <f t="shared" si="33"/>
         <v>44809.527300000009</v>
       </c>
       <c r="W146" s="17">
-        <f>R146*P146</f>
+        <f t="shared" si="34"/>
         <v>11202.381825000002</v>
       </c>
       <c r="X146" s="7">
-        <f>S146*O146</f>
+        <f t="shared" si="35"/>
         <v>201642.87285000001</v>
       </c>
       <c r="Y146" s="7">
-        <f>T146*P146</f>
+        <f t="shared" si="36"/>
         <v>67214.29095000001</v>
       </c>
       <c r="Z146" s="15">
@@ -16625,23 +16619,23 @@
         <v>0.08</v>
       </c>
       <c r="U147" s="7">
-        <f>L147-(V147+W147+X147+Y147)</f>
+        <f t="shared" si="32"/>
         <v>2203449.4167299997</v>
       </c>
       <c r="V147" s="7">
-        <f>Q147*L147</f>
+        <f t="shared" si="33"/>
         <v>62840.78875</v>
       </c>
       <c r="W147" s="7">
-        <f>R147*P147</f>
+        <f t="shared" si="34"/>
         <v>49267.178379999998</v>
       </c>
       <c r="X147" s="7">
-        <f>S147*O147</f>
+        <f t="shared" si="35"/>
         <v>1005.4526199999999</v>
       </c>
       <c r="Y147" s="7">
-        <f>T147*P147</f>
+        <f t="shared" si="36"/>
         <v>197068.71351999999</v>
       </c>
       <c r="Z147" s="15">
@@ -16711,23 +16705,23 @@
         <v>0.08</v>
       </c>
       <c r="U148" s="7">
-        <f>L148-(V148+W148+X148+Y148)</f>
+        <f t="shared" si="32"/>
         <v>1535090.375</v>
       </c>
       <c r="V148" s="7">
-        <f>Q148*L148</f>
+        <f t="shared" si="33"/>
         <v>99917.125</v>
       </c>
       <c r="W148" s="7">
-        <f>R148*P148</f>
+        <f t="shared" si="34"/>
         <v>19983.425000000003</v>
       </c>
       <c r="X148" s="7">
-        <f>S148*O148</f>
+        <f t="shared" si="35"/>
         <v>81750.375</v>
       </c>
       <c r="Y148" s="7">
-        <f>T148*P148</f>
+        <f t="shared" si="36"/>
         <v>79933.700000000012</v>
       </c>
       <c r="Z148" s="15">
@@ -16797,23 +16791,23 @@
         <v>0.08</v>
       </c>
       <c r="U149" s="7">
-        <f>L149-(V149+W149+X149+Y149)</f>
+        <f t="shared" ref="U149:U180" si="37">L149-(V149+W149+X149+Y149)</f>
         <v>2503274.5237500002</v>
       </c>
       <c r="V149" s="7">
-        <f>Q149*L149</f>
+        <f t="shared" si="33"/>
         <v>176597.85</v>
       </c>
       <c r="W149" s="7">
-        <f>R149*P149</f>
+        <f t="shared" ref="W149:W180" si="38">R149*P149</f>
         <v>38262.8675</v>
       </c>
       <c r="X149" s="7">
-        <f>S149*O149</f>
+        <f t="shared" si="35"/>
         <v>72110.788749999992</v>
       </c>
       <c r="Y149" s="7">
-        <f>T149*P149</f>
+        <f t="shared" si="36"/>
         <v>153051.47</v>
       </c>
       <c r="Z149" s="15">
@@ -16883,23 +16877,23 @@
         <v>0.08</v>
       </c>
       <c r="U150" s="7">
-        <f>L150-(V150+W150+X150+Y150)</f>
+        <f t="shared" si="37"/>
         <v>1736086.624416</v>
       </c>
       <c r="V150" s="7">
-        <f>Q150*L150</f>
+        <f t="shared" si="33"/>
         <v>122604.98759999999</v>
       </c>
       <c r="W150" s="7">
-        <f>R150*P150</f>
+        <f t="shared" si="38"/>
         <v>21251.531183999999</v>
       </c>
       <c r="X150" s="7">
-        <f>S150*O150</f>
+        <f t="shared" si="35"/>
         <v>78467.192064000003</v>
       </c>
       <c r="Y150" s="7">
-        <f>T150*P150</f>
+        <f t="shared" si="36"/>
         <v>85006.124735999998</v>
       </c>
       <c r="Z150" s="15">
@@ -16967,23 +16961,23 @@
         <v>0.08</v>
       </c>
       <c r="U151" s="7">
-        <f>L151-(V151+W151+X151+Y151)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V151" s="7">
-        <f>Q151*L151</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="W151" s="7">
-        <f>R151*P151</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X151" s="7">
-        <f>S151*O151</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="Y151" s="7">
-        <f>T151*P151</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z151" s="15">
@@ -17053,23 +17047,23 @@
         <v>0.12</v>
       </c>
       <c r="U152" s="7">
-        <f>L152-(V152+W152+X152+Y152)</f>
+        <f t="shared" si="37"/>
         <v>6232.2</v>
       </c>
       <c r="V152" s="7">
-        <f>Q152*L152</f>
+        <f t="shared" si="33"/>
         <v>423</v>
       </c>
       <c r="W152" s="7">
-        <f>R152*P152</f>
+        <f t="shared" si="38"/>
         <v>42.300000000000011</v>
       </c>
       <c r="X152" s="7">
-        <f>S152*O152</f>
+        <f t="shared" si="35"/>
         <v>98.7</v>
       </c>
       <c r="Y152" s="7">
-        <f>T152*P152</f>
+        <f t="shared" si="36"/>
         <v>253.80000000000004</v>
       </c>
       <c r="Z152" s="15">
@@ -17139,23 +17133,23 @@
         <v>0.08</v>
       </c>
       <c r="U153" s="7">
-        <f>L153-(V153+W153+X153+Y153)</f>
+        <f t="shared" si="37"/>
         <v>662652.44495999999</v>
       </c>
       <c r="V153" s="7">
-        <f>Q153*L153</f>
+        <f t="shared" si="33"/>
         <v>46885.786200000002</v>
       </c>
       <c r="W153" s="7">
-        <f>R153*P153</f>
+        <f t="shared" si="38"/>
         <v>9377.1572400000005</v>
       </c>
       <c r="X153" s="7">
-        <f>S153*O153</f>
+        <f t="shared" si="35"/>
         <v>25005.752639999999</v>
       </c>
       <c r="Y153" s="7">
-        <f>T153*P153</f>
+        <f t="shared" si="36"/>
         <v>37508.628960000002</v>
       </c>
       <c r="Z153" s="15">
@@ -17221,16 +17215,16 @@
       </c>
       <c r="T154" s="50"/>
       <c r="U154" s="59">
-        <f>L154-(V154+W154+X154+Y154)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V154" s="59"/>
       <c r="W154" s="59">
-        <f>R154*P154</f>
+        <f t="shared" si="38"/>
         <v>3300000</v>
       </c>
       <c r="X154" s="7">
-        <f>S154*O154</f>
+        <f t="shared" ref="X154:X185" si="39">S154*O154</f>
         <v>0</v>
       </c>
       <c r="Y154" s="59"/>
@@ -17299,23 +17293,23 @@
         <v>0.12</v>
       </c>
       <c r="U155" s="7">
-        <f>L155-(V155+W155+X155+Y155)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V155" s="7">
-        <f>Q155*L155</f>
+        <f t="shared" ref="V155:V186" si="40">Q155*L155</f>
         <v>0</v>
       </c>
       <c r="W155" s="7">
-        <f>R155*P155</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X155" s="7">
-        <f>S155*O155</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y155" s="7">
-        <f>T155*P155</f>
+        <f t="shared" ref="Y155:Y186" si="41">T155*P155</f>
         <v>0</v>
       </c>
       <c r="Z155" s="15">
@@ -17385,23 +17379,23 @@
         <v>0.08</v>
       </c>
       <c r="U156" s="7">
-        <f>L156-(V156+W156+X156+Y156)</f>
+        <f t="shared" si="37"/>
         <v>1415960.1713399999</v>
       </c>
       <c r="V156" s="7">
-        <f>Q156*L156</f>
+        <f t="shared" si="40"/>
         <v>99018.193799999994</v>
       </c>
       <c r="W156" s="7">
-        <f>R156*P156</f>
+        <f t="shared" si="38"/>
         <v>23104.245220000001</v>
       </c>
       <c r="X156" s="7">
-        <f>S156*O156</f>
+        <f t="shared" si="39"/>
         <v>19803.638759999998</v>
       </c>
       <c r="Y156" s="7">
-        <f>T156*P156</f>
+        <f t="shared" si="41"/>
         <v>92416.980880000003</v>
       </c>
       <c r="Z156" s="15">
@@ -17471,23 +17465,23 @@
         <v>0.06</v>
       </c>
       <c r="U157" s="7">
-        <f>L157-(V157+W157+X157+Y157)</f>
+        <f t="shared" si="37"/>
         <v>370923.29759999999</v>
       </c>
       <c r="V157" s="7">
-        <f>Q157*L157</f>
+        <f t="shared" si="40"/>
         <v>25878.369599999998</v>
       </c>
       <c r="W157" s="7">
-        <f>R157*P157</f>
+        <f t="shared" si="38"/>
         <v>4313.0616</v>
       </c>
       <c r="X157" s="7">
-        <f>S157*O157</f>
+        <f t="shared" si="39"/>
         <v>17252.2464</v>
       </c>
       <c r="Y157" s="7">
-        <f>T157*P157</f>
+        <f t="shared" si="41"/>
         <v>12939.184799999999</v>
       </c>
       <c r="Z157" s="15">
@@ -17557,23 +17551,23 @@
         <v>0.12</v>
       </c>
       <c r="U158" s="7">
-        <f>L158-(V158+W158+X158+Y158)</f>
+        <f t="shared" si="37"/>
         <v>600345.39471999998</v>
       </c>
       <c r="V158" s="7">
-        <f>Q158*L158</f>
+        <f t="shared" si="40"/>
         <v>43320.1728</v>
       </c>
       <c r="W158" s="7">
-        <f>R158*P158</f>
+        <f t="shared" si="38"/>
         <v>7942.031680000001</v>
       </c>
       <c r="X158" s="7">
-        <f>S158*O158</f>
+        <f t="shared" si="39"/>
         <v>22743.090720000004</v>
       </c>
       <c r="Y158" s="7">
-        <f>T158*P158</f>
+        <f t="shared" si="41"/>
         <v>47652.19008</v>
       </c>
       <c r="Z158" s="15">
@@ -17643,23 +17637,23 @@
         <v>0.12</v>
       </c>
       <c r="U159" s="7">
-        <f>L159-(V159+W159+X159+Y159)</f>
+        <f t="shared" si="37"/>
         <v>12675</v>
       </c>
       <c r="V159" s="7">
-        <f>Q159*L159</f>
+        <f t="shared" si="40"/>
         <v>900</v>
       </c>
       <c r="W159" s="7">
-        <f>R159*P159</f>
+        <f t="shared" si="38"/>
         <v>75</v>
       </c>
       <c r="X159" s="7">
-        <f>S159*O159</f>
+        <f t="shared" si="39"/>
         <v>450</v>
       </c>
       <c r="Y159" s="7">
-        <f>T159*P159</f>
+        <f t="shared" si="41"/>
         <v>900</v>
       </c>
       <c r="Z159" s="15">
@@ -17727,23 +17721,23 @@
         <v>0.12</v>
       </c>
       <c r="U160" s="7">
-        <f>L160-(V160+W160+X160+Y160)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V160" s="7">
-        <f>Q160*L160</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W160" s="7">
-        <f>R160*P160</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X160" s="7">
-        <f>S160*O160</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y160" s="7">
-        <f>T160*P160</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z160" s="15">
@@ -17813,23 +17807,23 @@
         <v>0.08</v>
       </c>
       <c r="U161" s="7">
-        <f>L161-(V161+W161+X161+Y161)</f>
+        <f t="shared" si="37"/>
         <v>532757.679</v>
       </c>
       <c r="V161" s="7">
-        <f>Q161*L161</f>
+        <f t="shared" si="40"/>
         <v>38559.06</v>
       </c>
       <c r="W161" s="17">
-        <f>R161*P161</f>
+        <f t="shared" si="38"/>
         <v>1927.9530000000002</v>
       </c>
       <c r="X161" s="7">
-        <f>S161*O161</f>
+        <f t="shared" si="39"/>
         <v>53982.683999999994</v>
       </c>
       <c r="Y161" s="7">
-        <f>T161*P161</f>
+        <f t="shared" si="41"/>
         <v>15423.624000000002</v>
       </c>
       <c r="Z161" s="15">
@@ -17879,11 +17873,11 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="O162" s="7">
-        <f t="shared" ref="O162:O225" si="32">M162*L162</f>
+        <f t="shared" ref="O162:O225" si="42">M162*L162</f>
         <v>290664.42749999993</v>
       </c>
       <c r="P162" s="7">
-        <f t="shared" ref="P162:P225" si="33">N162*L162</f>
+        <f t="shared" ref="P162:P225" si="43">N162*L162</f>
         <v>355256.52250000002</v>
       </c>
       <c r="Q162" s="11">
@@ -17899,27 +17893,27 @@
         <v>0.08</v>
       </c>
       <c r="U162" s="7">
-        <f>L162-(V162+W162+X162+Y162)</f>
+        <f t="shared" si="37"/>
         <v>560013.46364999993</v>
       </c>
       <c r="V162" s="7">
-        <f>Q162*L162</f>
+        <f t="shared" si="40"/>
         <v>38755.256999999998</v>
       </c>
       <c r="W162" s="7">
-        <f>R162*P162</f>
+        <f t="shared" si="38"/>
         <v>7105.1304500000006</v>
       </c>
       <c r="X162" s="7">
-        <f>S162*O162</f>
+        <f t="shared" si="39"/>
         <v>11626.577099999997</v>
       </c>
       <c r="Y162" s="7">
-        <f>T162*P162</f>
+        <f t="shared" si="41"/>
         <v>28420.521800000002</v>
       </c>
       <c r="Z162" s="15">
-        <f t="shared" ref="Z162:Z225" si="34">X162+Y162</f>
+        <f t="shared" ref="Z162:Z225" si="44">X162+Y162</f>
         <v>40047.098899999997</v>
       </c>
     </row>
@@ -17963,11 +17957,11 @@
         <v>0.65</v>
       </c>
       <c r="O163" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P163" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q163" s="11">
@@ -17983,27 +17977,27 @@
         <v>0.12</v>
       </c>
       <c r="U163" s="7">
-        <f>L163-(V163+W163+X163+Y163)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V163" s="7">
-        <f>Q163*L163</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W163" s="7">
-        <f>R163*P163</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X163" s="7">
-        <f>S163*O163</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y163" s="7">
-        <f>T163*P163</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z163" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -18049,11 +18043,11 @@
         <v>0.1</v>
       </c>
       <c r="O164" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>96106.607999999993</v>
       </c>
       <c r="P164" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>10678.512000000001</v>
       </c>
       <c r="Q164" s="11">
@@ -18067,27 +18061,27 @@
         <v>0.1</v>
       </c>
       <c r="U164" s="7">
-        <f>L164-(V164+W164+X164+Y164)</f>
+        <f t="shared" si="37"/>
         <v>94504.831200000001</v>
       </c>
       <c r="V164" s="7">
-        <f>Q164*L164</f>
+        <f t="shared" si="40"/>
         <v>6407.1071999999995</v>
       </c>
       <c r="W164" s="7">
-        <f>R164*P164</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X164" s="7">
-        <f>S164*O164</f>
+        <f t="shared" si="39"/>
         <v>4805.3303999999998</v>
       </c>
       <c r="Y164" s="7">
-        <f>T164*P164</f>
+        <f t="shared" si="41"/>
         <v>1067.8512000000001</v>
       </c>
       <c r="Z164" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>5873.1815999999999</v>
       </c>
     </row>
@@ -18133,11 +18127,11 @@
         <v>1</v>
       </c>
       <c r="O165" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P165" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>67748.75</v>
       </c>
       <c r="Q165" s="18">
@@ -18151,27 +18145,27 @@
         <v>0.25</v>
       </c>
       <c r="U165" s="7">
-        <f>L165-(V165+W165+X165+Y165)</f>
+        <f t="shared" si="37"/>
         <v>46746.637499999997</v>
       </c>
       <c r="V165" s="7">
-        <f>Q165*L165</f>
+        <f t="shared" si="40"/>
         <v>4064.9249999999997</v>
       </c>
       <c r="W165" s="7">
-        <f>R165*P165</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X165" s="7">
-        <f>S165*O165</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y165" s="7">
-        <f>T165*P165</f>
+        <f t="shared" si="41"/>
         <v>16937.1875</v>
       </c>
       <c r="Z165" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>16937.1875</v>
       </c>
     </row>
@@ -18215,11 +18209,11 @@
         <v>0.1</v>
       </c>
       <c r="O166" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P166" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q166" s="11">
@@ -18233,27 +18227,27 @@
         <v>0.25</v>
       </c>
       <c r="U166" s="7">
-        <f>L166-(V166+W166+X166+Y166)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V166" s="7">
-        <f>Q166*L166</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W166" s="7">
-        <f>R166*P166</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X166" s="7">
-        <f>S166*O166</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y166" s="7">
-        <f>T166*P166</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z166" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -18297,11 +18291,11 @@
         <v>0.1</v>
       </c>
       <c r="O167" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P167" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q167" s="11">
@@ -18315,27 +18309,27 @@
         <v>0.25</v>
       </c>
       <c r="U167" s="7">
-        <f>L167-(V167+W167+X167+Y167)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V167" s="7">
-        <f>Q167*L167</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W167" s="7">
-        <f>R167*P167</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X167" s="7">
-        <f>S167*O167</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y167" s="7">
-        <f>T167*P167</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z167" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -18379,11 +18373,11 @@
         <v>0.1</v>
       </c>
       <c r="O168" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P168" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q168" s="11">
@@ -18397,27 +18391,27 @@
         <v>0.25</v>
       </c>
       <c r="U168" s="7">
-        <f>L168-(V168+W168+X168+Y168)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V168" s="7">
-        <f>Q168*L168</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W168" s="7">
-        <f>R168*P168</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X168" s="7">
-        <f>S168*O168</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y168" s="7">
-        <f>T168*P168</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z168" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -18461,11 +18455,11 @@
         <v>0.1</v>
       </c>
       <c r="O169" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P169" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q169" s="11">
@@ -18479,27 +18473,27 @@
         <v>0.25</v>
       </c>
       <c r="U169" s="7">
-        <f>L169-(V169+W169+X169+Y169)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V169" s="7">
-        <f>Q169*L169</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W169" s="7">
-        <f>R169*P169</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X169" s="7">
-        <f>S169*O169</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y169" s="7">
-        <f>T169*P169</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z169" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -18545,11 +18539,11 @@
         <v>0.1</v>
       </c>
       <c r="O170" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>16650</v>
       </c>
       <c r="P170" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>1850</v>
       </c>
       <c r="Q170" s="11">
@@ -18563,27 +18557,27 @@
         <v>0.25</v>
       </c>
       <c r="U170" s="7">
-        <f>L170-(V170+W170+X170+Y170)</f>
+        <f t="shared" si="37"/>
         <v>14430</v>
       </c>
       <c r="V170" s="7">
-        <f>Q170*L170</f>
+        <f t="shared" si="40"/>
         <v>1110</v>
       </c>
       <c r="W170" s="7">
-        <f>R170*P170</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X170" s="7">
-        <f>S170*O170</f>
+        <f t="shared" si="39"/>
         <v>2497.5</v>
       </c>
       <c r="Y170" s="7">
-        <f>T170*P170</f>
+        <f t="shared" si="41"/>
         <v>462.5</v>
       </c>
       <c r="Z170" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>2960</v>
       </c>
     </row>
@@ -18627,11 +18621,11 @@
         <v>0.1</v>
       </c>
       <c r="O171" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P171" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q171" s="11">
@@ -18645,27 +18639,27 @@
         <v>0.25</v>
       </c>
       <c r="U171" s="7">
-        <f>L171-(V171+W171+X171+Y171)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V171" s="7">
-        <f>Q171*L171</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W171" s="7">
-        <f>R171*P171</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X171" s="7">
-        <f>S171*O171</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y171" s="7">
-        <f>T171*P171</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z171" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -18709,11 +18703,11 @@
         <v>0.1</v>
       </c>
       <c r="O172" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P172" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q172" s="11">
@@ -18727,27 +18721,27 @@
         <v>0.25</v>
       </c>
       <c r="U172" s="7">
-        <f>L172-(V172+W172+X172+Y172)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V172" s="7">
-        <f>Q172*L172</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W172" s="7">
-        <f>R172*P172</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X172" s="7">
-        <f>S172*O172</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y172" s="7">
-        <f>T172*P172</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z172" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -18793,11 +18787,11 @@
         <v>0.1</v>
       </c>
       <c r="O173" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>10234.800000000001</v>
       </c>
       <c r="P173" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>1137.2</v>
       </c>
       <c r="Q173" s="11">
@@ -18811,27 +18805,27 @@
         <v>0.25</v>
       </c>
       <c r="U173" s="7">
-        <f>L173-(V173+W173+X173+Y173)</f>
+        <f t="shared" si="37"/>
         <v>8870.16</v>
       </c>
       <c r="V173" s="7">
-        <f>Q173*L173</f>
+        <f t="shared" si="40"/>
         <v>682.31999999999994</v>
       </c>
       <c r="W173" s="7">
-        <f>R173*P173</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X173" s="7">
-        <f>S173*O173</f>
+        <f t="shared" si="39"/>
         <v>1535.22</v>
       </c>
       <c r="Y173" s="7">
-        <f>T173*P173</f>
+        <f t="shared" si="41"/>
         <v>284.3</v>
       </c>
       <c r="Z173" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>1819.52</v>
       </c>
     </row>
@@ -18877,11 +18871,11 @@
         <v>0.1</v>
       </c>
       <c r="O174" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>36809.1</v>
       </c>
       <c r="P174" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>4089.9</v>
       </c>
       <c r="Q174" s="11">
@@ -18895,27 +18889,27 @@
         <v>0.25</v>
       </c>
       <c r="U174" s="7">
-        <f>L174-(V174+W174+X174+Y174)</f>
+        <f t="shared" si="37"/>
         <v>31901.22</v>
       </c>
       <c r="V174" s="7">
-        <f>Q174*L174</f>
+        <f t="shared" si="40"/>
         <v>2453.94</v>
       </c>
       <c r="W174" s="7">
-        <f>R174*P174</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X174" s="7">
-        <f>S174*O174</f>
+        <f t="shared" si="39"/>
         <v>5521.3649999999998</v>
       </c>
       <c r="Y174" s="7">
-        <f>T174*P174</f>
+        <f t="shared" si="41"/>
         <v>1022.475</v>
       </c>
       <c r="Z174" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>6543.84</v>
       </c>
     </row>
@@ -18959,11 +18953,11 @@
         <v>0.1</v>
       </c>
       <c r="O175" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P175" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q175" s="11">
@@ -18977,27 +18971,27 @@
         <v>0.25</v>
       </c>
       <c r="U175" s="7">
-        <f>L175-(V175+W175+X175+Y175)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V175" s="7">
-        <f>Q175*L175</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W175" s="7">
-        <f>R175*P175</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X175" s="7">
-        <f>S175*O175</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y175" s="7">
-        <f>T175*P175</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z175" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -19041,11 +19035,11 @@
         <v>0.1</v>
       </c>
       <c r="O176" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P176" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q176" s="11">
@@ -19059,27 +19053,27 @@
         <v>0.25</v>
       </c>
       <c r="U176" s="7">
-        <f>L176-(V176+W176+X176+Y176)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V176" s="7">
-        <f>Q176*L176</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W176" s="7">
-        <f>R176*P176</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X176" s="7">
-        <f>S176*O176</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y176" s="7">
-        <f>T176*P176</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z176" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -19125,11 +19119,11 @@
         <v>0.1</v>
       </c>
       <c r="O177" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>19035</v>
       </c>
       <c r="P177" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>2115</v>
       </c>
       <c r="Q177" s="11">
@@ -19143,27 +19137,27 @@
         <v>0.25</v>
       </c>
       <c r="U177" s="7">
-        <f>L177-(V177+W177+X177+Y177)</f>
+        <f t="shared" si="37"/>
         <v>16497</v>
       </c>
       <c r="V177" s="7">
-        <f>Q177*L177</f>
+        <f t="shared" si="40"/>
         <v>1269</v>
       </c>
       <c r="W177" s="7">
-        <f>R177*P177</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X177" s="7">
-        <f>S177*O177</f>
+        <f t="shared" si="39"/>
         <v>2855.25</v>
       </c>
       <c r="Y177" s="7">
-        <f>T177*P177</f>
+        <f t="shared" si="41"/>
         <v>528.75</v>
       </c>
       <c r="Z177" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>3384</v>
       </c>
     </row>
@@ -19209,11 +19203,11 @@
         <v>0.1</v>
       </c>
       <c r="O178" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>451553.83199999999</v>
       </c>
       <c r="P178" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>50172.648000000001</v>
       </c>
       <c r="Q178" s="11">
@@ -19227,27 +19221,27 @@
         <v>0.23</v>
       </c>
       <c r="U178" s="7">
-        <f>L178-(V178+W178+X178+Y178)</f>
+        <f t="shared" si="37"/>
         <v>365256.87743999995</v>
       </c>
       <c r="V178" s="7">
-        <f>Q178*L178</f>
+        <f t="shared" si="40"/>
         <v>30103.588799999998</v>
       </c>
       <c r="W178" s="7">
-        <f>R178*P178</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X178" s="17">
-        <f>S178*O178</f>
+        <f t="shared" si="39"/>
         <v>94826.30472</v>
       </c>
       <c r="Y178" s="7">
-        <f>T178*P178</f>
+        <f t="shared" si="41"/>
         <v>11539.709040000002</v>
       </c>
       <c r="Z178" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>106366.01376</v>
       </c>
     </row>
@@ -19291,11 +19285,11 @@
         <v>0.1</v>
       </c>
       <c r="O179" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P179" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q179" s="11">
@@ -19309,27 +19303,27 @@
         <v>0.25</v>
       </c>
       <c r="U179" s="7">
-        <f>L179-(V179+W179+X179+Y179)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V179" s="7">
-        <f>Q179*L179</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W179" s="7">
-        <f>R179*P179</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X179" s="7">
-        <f>S179*O179</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y179" s="7">
-        <f>T179*P179</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z179" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -19375,11 +19369,11 @@
         <v>0.1</v>
       </c>
       <c r="O180" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>209006.685</v>
       </c>
       <c r="P180" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>23222.965</v>
       </c>
       <c r="Q180" s="11">
@@ -19393,27 +19387,27 @@
         <v>0.18</v>
       </c>
       <c r="U180" s="7">
-        <f>L180-(V180+W180+X180+Y180)</f>
+        <f t="shared" si="37"/>
         <v>182764.73454999999</v>
       </c>
       <c r="V180" s="7">
-        <f>Q180*L180</f>
+        <f t="shared" si="40"/>
         <v>13933.778999999999</v>
       </c>
       <c r="W180" s="7">
-        <f>R180*P180</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="X180" s="17">
-        <f>S180*O180</f>
+        <f t="shared" si="39"/>
         <v>31351.00275</v>
       </c>
       <c r="Y180" s="7">
-        <f>T180*P180</f>
+        <f t="shared" si="41"/>
         <v>4180.1337000000003</v>
       </c>
       <c r="Z180" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>35531.136449999998</v>
       </c>
     </row>
@@ -19459,11 +19453,11 @@
         <v>0.1</v>
       </c>
       <c r="O181" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>3906</v>
       </c>
       <c r="P181" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>434</v>
       </c>
       <c r="Q181" s="11">
@@ -19477,27 +19471,27 @@
         <v>0.25</v>
       </c>
       <c r="U181" s="7">
-        <f>L181-(V181+W181+X181+Y181)</f>
+        <f t="shared" ref="U181:U212" si="45">L181-(V181+W181+X181+Y181)</f>
         <v>3385.2</v>
       </c>
       <c r="V181" s="7">
-        <f>Q181*L181</f>
+        <f t="shared" si="40"/>
         <v>260.39999999999998</v>
       </c>
       <c r="W181" s="7">
-        <f>R181*P181</f>
+        <f t="shared" ref="W181:W212" si="46">R181*P181</f>
         <v>0</v>
       </c>
       <c r="X181" s="7">
-        <f>S181*O181</f>
+        <f t="shared" si="39"/>
         <v>585.9</v>
       </c>
       <c r="Y181" s="7">
-        <f>T181*P181</f>
+        <f t="shared" si="41"/>
         <v>108.5</v>
       </c>
       <c r="Z181" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>694.4</v>
       </c>
     </row>
@@ -19541,11 +19535,11 @@
         <v>0.1</v>
       </c>
       <c r="O182" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P182" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q182" s="11">
@@ -19559,27 +19553,27 @@
         <v>0.25</v>
       </c>
       <c r="U182" s="7">
-        <f>L182-(V182+W182+X182+Y182)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V182" s="7">
-        <f>Q182*L182</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W182" s="7">
-        <f>R182*P182</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X182" s="7">
-        <f>S182*O182</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y182" s="7">
-        <f>T182*P182</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z182" s="26">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -19625,11 +19619,11 @@
         <v>1</v>
       </c>
       <c r="O183" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P183" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>1503081.81</v>
       </c>
       <c r="Q183" s="18">
@@ -19643,27 +19637,27 @@
         <v>0.18</v>
       </c>
       <c r="U183" s="7">
-        <f>L183-(V183+W183+X183+Y183)</f>
+        <f t="shared" si="45"/>
         <v>1112280.5394000001</v>
       </c>
       <c r="V183" s="7">
-        <f>Q183*L183</f>
+        <f t="shared" si="40"/>
         <v>90184.908599999995</v>
       </c>
       <c r="W183" s="28">
-        <f>R183*P183</f>
+        <f t="shared" si="46"/>
         <v>30061.636200000001</v>
       </c>
       <c r="X183" s="7">
-        <f>S183*O183</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y183" s="7">
-        <f>T183*P183</f>
+        <f t="shared" si="41"/>
         <v>270554.72580000001</v>
       </c>
       <c r="Z183" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>270554.72580000001</v>
       </c>
     </row>
@@ -19709,11 +19703,11 @@
         <v>0.2</v>
       </c>
       <c r="O184" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>243813.41600000003</v>
       </c>
       <c r="P184" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>60953.354000000007</v>
       </c>
       <c r="Q184" s="11">
@@ -19727,27 +19721,27 @@
         <v>0.1</v>
       </c>
       <c r="U184" s="7">
-        <f>L184-(V184+W184+X184+Y184)</f>
+        <f t="shared" si="45"/>
         <v>258442.22096000001</v>
       </c>
       <c r="V184" s="7">
-        <f>Q184*L184</f>
+        <f t="shared" si="40"/>
         <v>18286.0062</v>
       </c>
       <c r="W184" s="7">
-        <f>R184*P184</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X184" s="7">
-        <f>S184*O184</f>
+        <f t="shared" si="39"/>
         <v>21943.207440000002</v>
       </c>
       <c r="Y184" s="7">
-        <f>T184*P184</f>
+        <f t="shared" si="41"/>
         <v>6095.3354000000008</v>
       </c>
       <c r="Z184" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>28038.542840000002</v>
       </c>
     </row>
@@ -19791,11 +19785,11 @@
         <v>0</v>
       </c>
       <c r="O185" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P185" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q185" s="11">
@@ -19807,27 +19801,27 @@
       </c>
       <c r="T185" s="11"/>
       <c r="U185" s="7">
-        <f>L185-(V185+W185+X185+Y185)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V185" s="7">
-        <f>Q185*L185</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W185" s="7">
-        <f>R185*P185</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X185" s="7">
-        <f>S185*O185</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y185" s="7">
-        <f>T185*P185</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z185" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -19871,11 +19865,11 @@
         <v>0.2</v>
       </c>
       <c r="O186" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P186" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q186" s="11">
@@ -19891,27 +19885,27 @@
         <v>0.6</v>
       </c>
       <c r="U186" s="7">
-        <f>L186-(V186+W186+X186+Y186)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V186" s="7">
-        <f>Q186*L186</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W186" s="7">
-        <f>R186*P186</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X186" s="7">
-        <f>S186*O186</f>
+        <f t="shared" ref="X186:X217" si="47">S186*O186</f>
         <v>0</v>
       </c>
       <c r="Y186" s="7">
-        <f>T186*P186</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z186" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -19957,11 +19951,11 @@
         <v>0.5</v>
       </c>
       <c r="O187" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>212621.89</v>
       </c>
       <c r="P187" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>212621.89</v>
       </c>
       <c r="Q187" s="11">
@@ -19977,27 +19971,27 @@
         <v>0.4</v>
       </c>
       <c r="U187" s="7">
-        <f>L187-(V187+W187+X187+Y187)</f>
+        <f t="shared" si="45"/>
         <v>250893.83020000003</v>
       </c>
       <c r="V187" s="7">
-        <f>Q187*L187</f>
+        <f t="shared" ref="V187:V218" si="48">Q187*L187</f>
         <v>25514.626800000002</v>
       </c>
       <c r="W187" s="7">
-        <f>R187*P187</f>
+        <f t="shared" si="46"/>
         <v>42524.378000000004</v>
       </c>
       <c r="X187" s="7">
-        <f>S187*O187</f>
+        <f t="shared" si="47"/>
         <v>21262.189000000002</v>
       </c>
       <c r="Y187" s="7">
-        <f>T187*P187</f>
+        <f t="shared" ref="Y187:Y218" si="49">T187*P187</f>
         <v>85048.756000000008</v>
       </c>
       <c r="Z187" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>106310.94500000001</v>
       </c>
     </row>
@@ -20043,11 +20037,11 @@
         <v>0.2</v>
       </c>
       <c r="O188" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>145392.80000000002</v>
       </c>
       <c r="P188" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>36348.200000000004</v>
       </c>
       <c r="Q188" s="11">
@@ -20061,27 +20055,27 @@
         <v>0.1</v>
       </c>
       <c r="U188" s="7">
-        <f>L188-(V188+W188+X188+Y188)</f>
+        <f t="shared" si="45"/>
         <v>152662.44</v>
       </c>
       <c r="V188" s="7">
-        <f>Q188*L188</f>
+        <f t="shared" si="48"/>
         <v>10904.46</v>
       </c>
       <c r="W188" s="7">
-        <f>R188*P188</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X188" s="7">
-        <f>S188*O188</f>
+        <f t="shared" si="47"/>
         <v>14539.280000000002</v>
       </c>
       <c r="Y188" s="7">
-        <f>T188*P188</f>
+        <f t="shared" si="49"/>
         <v>3634.8200000000006</v>
       </c>
       <c r="Z188" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>18174.100000000002</v>
       </c>
     </row>
@@ -20125,11 +20119,11 @@
         <v>0.5</v>
       </c>
       <c r="O189" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P189" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q189" s="11">
@@ -20143,27 +20137,27 @@
         <v>0.1</v>
       </c>
       <c r="U189" s="7">
-        <f>L189-(V189+W189+X189+Y189)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V189" s="7">
-        <f>Q189*L189</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W189" s="7">
-        <f>R189*P189</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X189" s="7">
-        <f>S189*O189</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y189" s="7">
-        <f>T189*P189</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z189" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -20209,11 +20203,11 @@
         <v>0.5</v>
       </c>
       <c r="O190" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>345720.8</v>
       </c>
       <c r="P190" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>345720.8</v>
       </c>
       <c r="Q190" s="11">
@@ -20229,27 +20223,27 @@
         <v>0.3</v>
       </c>
       <c r="U190" s="7">
-        <f>L190-(V190+W190+X190+Y190)</f>
+        <f t="shared" si="45"/>
         <v>442522.62399999995</v>
       </c>
       <c r="V190" s="7">
-        <f>Q190*L190</f>
+        <f t="shared" si="48"/>
         <v>41486.495999999999</v>
       </c>
       <c r="W190" s="7">
-        <f>R190*P190</f>
+        <f t="shared" si="46"/>
         <v>69144.160000000003</v>
       </c>
       <c r="X190" s="7">
-        <f>S190*O190</f>
+        <f t="shared" si="47"/>
         <v>34572.080000000002</v>
       </c>
       <c r="Y190" s="7">
-        <f>T190*P190</f>
+        <f t="shared" si="49"/>
         <v>103716.23999999999</v>
       </c>
       <c r="Z190" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>138288.32000000001</v>
       </c>
     </row>
@@ -20293,11 +20287,11 @@
         <v>0.2</v>
       </c>
       <c r="O191" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P191" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q191" s="11">
@@ -20313,27 +20307,27 @@
         <v>0.6</v>
       </c>
       <c r="U191" s="7">
-        <f>L191-(V191+W191+X191+Y191)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V191" s="7">
-        <f>Q191*L191</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W191" s="7">
-        <f>R191*P191</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X191" s="7">
-        <f>S191*O191</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y191" s="7">
-        <f>T191*P191</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z191" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -20377,11 +20371,11 @@
         <v>0</v>
       </c>
       <c r="O192" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P192" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q192" s="11">
@@ -20393,27 +20387,27 @@
       </c>
       <c r="T192" s="11"/>
       <c r="U192" s="7">
-        <f>L192-(V192+W192+X192+Y192)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V192" s="7">
-        <f>Q192*L192</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W192" s="7">
-        <f>R192*P192</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X192" s="7">
-        <f>S192*O192</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y192" s="7">
-        <f>T192*P192</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z192" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -20457,11 +20451,11 @@
         <v>0</v>
       </c>
       <c r="O193" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P193" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q193" s="11">
@@ -20473,27 +20467,27 @@
       </c>
       <c r="T193" s="11"/>
       <c r="U193" s="7">
-        <f>L193-(V193+W193+X193+Y193)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V193" s="7">
-        <f>Q193*L193</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W193" s="7">
-        <f>R193*P193</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X193" s="7">
-        <f>S193*O193</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y193" s="7">
-        <f>T193*P193</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z193" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -20539,11 +20533,11 @@
         <v>0</v>
       </c>
       <c r="O194" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>500</v>
       </c>
       <c r="P194" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q194" s="11">
@@ -20555,27 +20549,27 @@
       </c>
       <c r="T194" s="11"/>
       <c r="U194" s="7">
-        <f>L194-(V194+W194+X194+Y194)</f>
+        <f t="shared" si="45"/>
         <v>430</v>
       </c>
       <c r="V194" s="7">
-        <f>Q194*L194</f>
+        <f t="shared" si="48"/>
         <v>30</v>
       </c>
       <c r="W194" s="7">
-        <f>R194*P194</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X194" s="7">
-        <f>S194*O194</f>
+        <f t="shared" si="47"/>
         <v>40</v>
       </c>
       <c r="Y194" s="7">
-        <f>T194*P194</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z194" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>40</v>
       </c>
     </row>
@@ -20619,11 +20613,11 @@
         <v>0</v>
       </c>
       <c r="O195" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P195" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q195" s="11">
@@ -20635,27 +20629,27 @@
       </c>
       <c r="T195" s="11"/>
       <c r="U195" s="7">
-        <f>L195-(V195+W195+X195+Y195)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V195" s="7">
-        <f>Q195*L195</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W195" s="7">
-        <f>R195*P195</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X195" s="7">
-        <f>S195*O195</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y195" s="7">
-        <f>T195*P195</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z195" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -20699,11 +20693,11 @@
         <v>0.3</v>
       </c>
       <c r="O196" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P196" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q196" s="11">
@@ -20717,27 +20711,27 @@
         <v>0.3</v>
       </c>
       <c r="U196" s="7">
-        <f>L196-(V196+W196+X196+Y196)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V196" s="7">
-        <f>Q196*L196</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W196" s="7">
-        <f>R196*P196</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X196" s="7">
-        <f>S196*O196</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y196" s="7">
-        <f>T196*P196</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z196" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -20781,11 +20775,11 @@
         <v>0</v>
       </c>
       <c r="O197" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P197" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q197" s="11">
@@ -20797,27 +20791,27 @@
       </c>
       <c r="T197" s="11"/>
       <c r="U197" s="7">
-        <f>L197-(V197+W197+X197+Y197)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V197" s="7">
-        <f>Q197*L197</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W197" s="7">
-        <f>R197*P197</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X197" s="7">
-        <f>S197*O197</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y197" s="7">
-        <f>T197*P197</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z197" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -20861,11 +20855,11 @@
         <v>0.3</v>
       </c>
       <c r="O198" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P198" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q198" s="11">
@@ -20879,27 +20873,27 @@
         <v>0.3</v>
       </c>
       <c r="U198" s="7">
-        <f>L198-(V198+W198+X198+Y198)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V198" s="7">
-        <f>Q198*L198</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W198" s="7">
-        <f>R198*P198</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X198" s="7">
-        <f>S198*O198</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y198" s="7">
-        <f>T198*P198</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z198" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -20943,11 +20937,11 @@
         <v>0</v>
       </c>
       <c r="O199" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P199" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q199" s="11">
@@ -20957,27 +20951,27 @@
       <c r="S199" s="11"/>
       <c r="T199" s="11"/>
       <c r="U199" s="7">
-        <f>L199-(V199+W199+X199+Y199)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V199" s="7">
-        <f>Q199*L199</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W199" s="7">
-        <f>R199*P199</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X199" s="7">
-        <f>S199*O199</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y199" s="7">
-        <f>T199*P199</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z199" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -21021,11 +21015,11 @@
         <v>0.3</v>
       </c>
       <c r="O200" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P200" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q200" s="11">
@@ -21039,27 +21033,27 @@
         <v>0.15</v>
       </c>
       <c r="U200" s="7">
-        <f>L200-(V200+W200+X200+Y200)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V200" s="7">
-        <f>Q200*L200</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W200" s="7">
-        <f>R200*P200</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X200" s="7">
-        <f>S200*O200</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y200" s="7">
-        <f>T200*P200</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z200" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -21103,11 +21097,11 @@
         <v>0</v>
       </c>
       <c r="O201" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P201" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q201" s="11">
@@ -21119,27 +21113,27 @@
       </c>
       <c r="T201" s="11"/>
       <c r="U201" s="7">
-        <f>L201-(V201+W201+X201+Y201)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V201" s="7">
-        <f>Q201*L201</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W201" s="7">
-        <f>R201*P201</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X201" s="7">
-        <f>S201*O201</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y201" s="7">
-        <f>T201*P201</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z201" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -21183,11 +21177,11 @@
         <v>0</v>
       </c>
       <c r="O202" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P202" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q202" s="11">
@@ -21199,27 +21193,27 @@
       </c>
       <c r="T202" s="11"/>
       <c r="U202" s="7">
-        <f>L202-(V202+W202+X202+Y202)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V202" s="7">
-        <f>Q202*L202</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W202" s="7">
-        <f>R202*P202</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X202" s="7">
-        <f>S202*O202</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y202" s="7">
-        <f>T202*P202</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z202" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -21263,11 +21257,11 @@
         <v>0.1</v>
       </c>
       <c r="O203" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P203" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q203" s="11">
@@ -21281,27 +21275,27 @@
         <v>0</v>
       </c>
       <c r="U203" s="7">
-        <f>L203-(V203+W203+X203+Y203)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V203" s="7">
-        <f>Q203*L203</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W203" s="7">
-        <f>R203*P203</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X203" s="7">
-        <f>S203*O203</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y203" s="7">
-        <f>T203*P203</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z203" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -21345,11 +21339,11 @@
         <v>0</v>
       </c>
       <c r="O204" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P204" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q204" s="11">
@@ -21361,27 +21355,27 @@
       </c>
       <c r="T204" s="11"/>
       <c r="U204" s="7">
-        <f>L204-(V204+W204+X204+Y204)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V204" s="7">
-        <f>Q204*L204</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W204" s="7">
-        <f>R204*P204</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X204" s="7">
-        <f>S204*O204</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y204" s="7">
-        <f>T204*P204</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z204" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -21427,11 +21421,11 @@
         <v>0.5</v>
       </c>
       <c r="O205" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>22335.5</v>
       </c>
       <c r="P205" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>22335.5</v>
       </c>
       <c r="Q205" s="11">
@@ -21445,27 +21439,27 @@
         <v>0</v>
       </c>
       <c r="U205" s="7">
-        <f>L205-(V205+W205+X205+Y205)</f>
+        <f t="shared" si="45"/>
         <v>39757.19</v>
       </c>
       <c r="V205" s="7">
-        <f>Q205*L205</f>
+        <f t="shared" si="48"/>
         <v>2680.2599999999998</v>
       </c>
       <c r="W205" s="7">
-        <f>R205*P205</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X205" s="7">
-        <f>S205*O205</f>
+        <f t="shared" si="47"/>
         <v>2233.5500000000002</v>
       </c>
       <c r="Y205" s="7">
-        <f>T205*P205</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z205" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>2233.5500000000002</v>
       </c>
     </row>
@@ -21509,11 +21503,11 @@
         <v>0</v>
       </c>
       <c r="O206" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P206" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q206" s="11">
@@ -21525,27 +21519,27 @@
       </c>
       <c r="T206" s="11"/>
       <c r="U206" s="7">
-        <f>L206-(V206+W206+X206+Y206)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V206" s="7">
-        <f>Q206*L206</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W206" s="7">
-        <f>R206*P206</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X206" s="7">
-        <f>S206*O206</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y206" s="7">
-        <f>T206*P206</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z206" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -21589,11 +21583,11 @@
         <v>0</v>
       </c>
       <c r="O207" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P207" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q207" s="11">
@@ -21605,27 +21599,27 @@
       </c>
       <c r="T207" s="33"/>
       <c r="U207" s="7">
-        <f>L207-(V207+W207+X207+Y207)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V207" s="7">
-        <f>Q207*L207</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W207" s="7">
-        <f>R207*P207</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X207" s="7">
-        <f>S207*O207</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y207" s="7">
-        <f>T207*P207</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z207" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -21669,11 +21663,11 @@
         <v>0</v>
       </c>
       <c r="O208" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P208" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q208" s="11">
@@ -21685,27 +21679,27 @@
       </c>
       <c r="T208" s="11"/>
       <c r="U208" s="7">
-        <f>L208-(V208+W208+X208+Y208)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V208" s="7">
-        <f>Q208*L208</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W208" s="7">
-        <f>R208*P208</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X208" s="7">
-        <f>S208*O208</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y208" s="7">
-        <f>T208*P208</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z208" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -21749,11 +21743,11 @@
         <v>0.1</v>
       </c>
       <c r="O209" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P209" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q209" s="11">
@@ -21767,27 +21761,27 @@
         <v>0.25</v>
       </c>
       <c r="U209" s="7">
-        <f>L209-(V209+W209+X209+Y209)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V209" s="7">
-        <f>Q209*L209</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W209" s="7">
-        <f>R209*P209</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X209" s="7">
-        <f>S209*O209</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y209" s="7">
-        <f>T209*P209</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z209" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -21831,11 +21825,11 @@
         <v>0.1</v>
       </c>
       <c r="O210" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P210" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q210" s="11">
@@ -21849,27 +21843,27 @@
         <v>0.3</v>
       </c>
       <c r="U210" s="7">
-        <f>L210-(V210+W210+X210+Y210)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V210" s="7">
-        <f>Q210*L210</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W210" s="7">
-        <f>R210*P210</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X210" s="7">
-        <f>S210*O210</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y210" s="7">
-        <f>T210*P210</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z210" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -21913,11 +21907,11 @@
         <v>0.1</v>
       </c>
       <c r="O211" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P211" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q211" s="11">
@@ -21931,27 +21925,27 @@
         <v>0.25</v>
       </c>
       <c r="U211" s="7">
-        <f>L211-(V211+W211+X211+Y211)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V211" s="7">
-        <f>Q211*L211</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W211" s="7">
-        <f>R211*P211</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X211" s="7">
-        <f>S211*O211</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y211" s="7">
-        <f>T211*P211</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z211" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -21995,11 +21989,11 @@
         <v>0.1</v>
       </c>
       <c r="O212" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P212" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q212" s="11">
@@ -22013,27 +22007,27 @@
         <v>1</v>
       </c>
       <c r="U212" s="7">
-        <f>L212-(V212+W212+X212+Y212)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V212" s="7">
-        <f>Q212*L212</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W212" s="7">
-        <f>R212*P212</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X212" s="7">
-        <f>S212*O212</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y212" s="7">
-        <f>T212*P212</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z212" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -22077,11 +22071,11 @@
         <v>0</v>
       </c>
       <c r="O213" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P213" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q213" s="11">
@@ -22093,27 +22087,27 @@
       </c>
       <c r="T213" s="11"/>
       <c r="U213" s="7">
-        <f>L213-(V213+W213+X213+Y213)</f>
+        <f t="shared" ref="U213:U244" si="50">L213-(V213+W213+X213+Y213)</f>
         <v>0</v>
       </c>
       <c r="V213" s="7">
-        <f>Q213*L213</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W213" s="7">
-        <f>R213*P213</f>
+        <f t="shared" ref="W213:W230" si="51">R213*P213</f>
         <v>0</v>
       </c>
       <c r="X213" s="7">
-        <f>S213*O213</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y213" s="7">
-        <f>T213*P213</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z213" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -22159,11 +22153,11 @@
         <v>0.2</v>
       </c>
       <c r="O214" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>10629.6</v>
       </c>
       <c r="P214" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>2657.4</v>
       </c>
       <c r="Q214" s="11">
@@ -22177,27 +22171,27 @@
         <v>0.1</v>
       </c>
       <c r="U214" s="7">
-        <f>L214-(V214+W214+X214+Y214)</f>
+        <f t="shared" si="50"/>
         <v>11692.56</v>
       </c>
       <c r="V214" s="7">
-        <f>Q214*L214</f>
+        <f t="shared" si="48"/>
         <v>797.22</v>
       </c>
       <c r="W214" s="7">
-        <f>R214*P214</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X214" s="7">
-        <f>S214*O214</f>
+        <f t="shared" si="47"/>
         <v>531.48</v>
       </c>
       <c r="Y214" s="7">
-        <f>T214*P214</f>
+        <f t="shared" si="49"/>
         <v>265.74</v>
       </c>
       <c r="Z214" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>797.22</v>
       </c>
     </row>
@@ -22241,11 +22235,11 @@
         <v>0.1</v>
       </c>
       <c r="O215" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P215" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q215" s="11">
@@ -22259,27 +22253,27 @@
         <v>0.25</v>
       </c>
       <c r="U215" s="7">
-        <f>L215-(V215+W215+X215+Y215)</f>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="V215" s="7">
-        <f>Q215*L215</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W215" s="7">
-        <f>R215*P215</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X215" s="7">
-        <f>S215*O215</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y215" s="7">
-        <f>T215*P215</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z215" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -22323,11 +22317,11 @@
         <v>0.1</v>
       </c>
       <c r="O216" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P216" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q216" s="11">
@@ -22341,27 +22335,27 @@
         <v>0.25</v>
       </c>
       <c r="U216" s="7">
-        <f>L216-(V216+W216+X216+Y216)</f>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="V216" s="7">
-        <f>Q216*L216</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W216" s="7">
-        <f>R216*P216</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X216" s="7">
-        <f>S216*O216</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y216" s="7">
-        <f>T216*P216</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z216" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -22405,11 +22399,11 @@
         <v>0.1</v>
       </c>
       <c r="O217" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P217" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q217" s="11">
@@ -22423,27 +22417,27 @@
         <v>0.1</v>
       </c>
       <c r="U217" s="7">
-        <f>L217-(V217+W217+X217+Y217)</f>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="V217" s="7">
-        <f>Q217*L217</f>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W217" s="7">
-        <f>R217*P217</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X217" s="7">
-        <f>S217*O217</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y217" s="7">
-        <f>T217*P217</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="Z217" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -22489,11 +22483,11 @@
         <v>0.3</v>
       </c>
       <c r="O218" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>13650.231</v>
       </c>
       <c r="P218" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>5850.0990000000002</v>
       </c>
       <c r="Q218" s="11">
@@ -22507,27 +22501,27 @@
         <v>0.01</v>
       </c>
       <c r="U218" s="7">
-        <f>L218-(V218+W218+X218+Y218)</f>
+        <f t="shared" si="50"/>
         <v>18135.306900000003</v>
       </c>
       <c r="V218" s="7">
-        <f>Q218*L218</f>
+        <f t="shared" si="48"/>
         <v>1170.0198</v>
       </c>
       <c r="W218" s="7">
-        <f>R218*P218</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X218" s="7">
-        <f>S218*O218</f>
+        <f t="shared" ref="X218:X230" si="52">S218*O218</f>
         <v>136.50230999999999</v>
       </c>
       <c r="Y218" s="7">
-        <f>T218*P218</f>
+        <f t="shared" si="49"/>
         <v>58.500990000000002</v>
       </c>
       <c r="Z218" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>195.0033</v>
       </c>
     </row>
@@ -22573,11 +22567,11 @@
         <v>0.3</v>
       </c>
       <c r="O219" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>262784.011</v>
       </c>
       <c r="P219" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>112621.719</v>
       </c>
       <c r="Q219" s="11">
@@ -22591,27 +22585,27 @@
         <v>0.01</v>
       </c>
       <c r="U219" s="7">
-        <f>L219-(V219+W219+X219+Y219)</f>
+        <f t="shared" si="50"/>
         <v>349127.32889999996</v>
       </c>
       <c r="V219" s="7">
-        <f>Q219*L219</f>
+        <f t="shared" ref="V219:V230" si="53">Q219*L219</f>
         <v>22524.343799999999</v>
       </c>
       <c r="W219" s="7">
-        <f>R219*P219</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X219" s="7">
-        <f>S219*O219</f>
+        <f t="shared" si="52"/>
         <v>2627.8401100000001</v>
       </c>
       <c r="Y219" s="7">
-        <f>T219*P219</f>
+        <f t="shared" ref="Y219:Y230" si="54">T219*P219</f>
         <v>1126.2171900000001</v>
       </c>
       <c r="Z219" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>3754.0573000000004</v>
       </c>
     </row>
@@ -22657,11 +22651,11 @@
         <v>1</v>
       </c>
       <c r="O220" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P220" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>4582268.16</v>
       </c>
       <c r="Q220" s="18">
@@ -22675,27 +22669,27 @@
         <v>0.3</v>
       </c>
       <c r="U220" s="7">
-        <f>L220-(V220+W220+X220+Y220)</f>
+        <f t="shared" si="50"/>
         <v>2153666.0351999998</v>
       </c>
       <c r="V220" s="7">
-        <f>Q220*L220</f>
+        <f t="shared" si="53"/>
         <v>274936.08960000001</v>
       </c>
       <c r="W220" s="28">
-        <f>R220*P220</f>
+        <f t="shared" si="51"/>
         <v>778985.58720000007</v>
       </c>
       <c r="X220" s="7">
-        <f>S220*O220</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="Y220" s="7">
-        <f>T220*P220</f>
+        <f t="shared" si="54"/>
         <v>1374680.4480000001</v>
       </c>
       <c r="Z220" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>1374680.4480000001</v>
       </c>
     </row>
@@ -22741,11 +22735,11 @@
         <v>0</v>
       </c>
       <c r="O221" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>31561.119999999999</v>
       </c>
       <c r="P221" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q221" s="11">
@@ -22757,27 +22751,27 @@
       </c>
       <c r="T221" s="11"/>
       <c r="U221" s="7">
-        <f>L221-(V221+W221+X221+Y221)</f>
+        <f t="shared" si="50"/>
         <v>28089.396799999999</v>
       </c>
       <c r="V221" s="7">
-        <f>Q221*L221</f>
+        <f t="shared" si="53"/>
         <v>1893.6671999999999</v>
       </c>
       <c r="W221" s="7">
-        <f>R221*P221</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X221" s="7">
-        <f>S221*O221</f>
+        <f t="shared" si="52"/>
         <v>1578.056</v>
       </c>
       <c r="Y221" s="7">
-        <f>T221*P221</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Z221" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>1578.056</v>
       </c>
     </row>
@@ -22821,11 +22815,11 @@
         <v>0</v>
       </c>
       <c r="O222" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P222" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q222" s="11">
@@ -22837,27 +22831,27 @@
       </c>
       <c r="T222" s="11"/>
       <c r="U222" s="7">
-        <f>L222-(V222+W222+X222+Y222)</f>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="V222" s="7">
-        <f>Q222*L222</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="W222" s="7">
-        <f>R222*P222</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X222" s="7">
-        <f>S222*O222</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="Y222" s="7">
-        <f>T222*P222</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Z222" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -22901,11 +22895,11 @@
         <v>0.1</v>
       </c>
       <c r="O223" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P223" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q223" s="11">
@@ -22919,27 +22913,27 @@
         <v>0.25</v>
       </c>
       <c r="U223" s="7">
-        <f>L223-(V223+W223+X223+Y223)</f>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="V223" s="7">
-        <f>Q223*L223</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="W223" s="7">
-        <f>R223*P223</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X223" s="7">
-        <f>S223*O223</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="Y223" s="7">
-        <f>T223*P223</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Z223" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -22983,11 +22977,11 @@
         <v>0.2</v>
       </c>
       <c r="O224" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P224" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Q224" s="11">
@@ -23001,27 +22995,27 @@
         <v>0.25</v>
       </c>
       <c r="U224" s="7">
-        <f>L224-(V224+W224+X224+Y224)</f>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="V224" s="7">
-        <f>Q224*L224</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="W224" s="7">
-        <f>R224*P224</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X224" s="7">
-        <f>S224*O224</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="Y224" s="7">
-        <f>T224*P224</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Z224" s="61">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
     </row>
@@ -23067,11 +23061,11 @@
         <v>0.2</v>
       </c>
       <c r="O225" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="42"/>
         <v>96</v>
       </c>
       <c r="P225" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="43"/>
         <v>24</v>
       </c>
       <c r="Q225" s="11">
@@ -23085,27 +23079,27 @@
         <v>0.25</v>
       </c>
       <c r="U225" s="7">
-        <f>L225-(V225+W225+X225+Y225)</f>
+        <f t="shared" si="50"/>
         <v>97.2</v>
       </c>
       <c r="V225" s="7">
-        <f>Q225*L225</f>
+        <f t="shared" si="53"/>
         <v>7.1999999999999993</v>
       </c>
       <c r="W225" s="7">
-        <f>R225*P225</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X225" s="7">
-        <f>S225*O225</f>
+        <f t="shared" si="52"/>
         <v>9.6000000000000014</v>
       </c>
       <c r="Y225" s="7">
-        <f>T225*P225</f>
+        <f t="shared" si="54"/>
         <v>6</v>
       </c>
       <c r="Z225" s="61">
-        <f t="shared" si="34"/>
+        <f t="shared" si="44"/>
         <v>15.600000000000001</v>
       </c>
     </row>
@@ -23151,11 +23145,11 @@
         <v>0.2</v>
       </c>
       <c r="O226" s="7">
-        <f t="shared" ref="O226:O230" si="35">M226*L226</f>
+        <f t="shared" ref="O226:O230" si="55">M226*L226</f>
         <v>91486.8</v>
       </c>
       <c r="P226" s="7">
-        <f t="shared" ref="P226:P230" si="36">N226*L226</f>
+        <f t="shared" ref="P226:P230" si="56">N226*L226</f>
         <v>22871.7</v>
       </c>
       <c r="Q226" s="11">
@@ -23169,27 +23163,27 @@
         <v>0.18</v>
       </c>
       <c r="U226" s="7">
-        <f>L226-(V226+W226+X226+Y226)</f>
+        <f t="shared" si="50"/>
         <v>89657.063999999998</v>
       </c>
       <c r="V226" s="7">
-        <f>Q226*L226</f>
+        <f t="shared" si="53"/>
         <v>6861.5099999999993</v>
       </c>
       <c r="W226" s="7">
-        <f>R226*P226</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X226" s="7">
-        <f>S226*O226</f>
+        <f t="shared" si="52"/>
         <v>13723.02</v>
       </c>
       <c r="Y226" s="7">
-        <f>T226*P226</f>
+        <f t="shared" si="54"/>
         <v>4116.9059999999999</v>
       </c>
       <c r="Z226" s="61">
-        <f t="shared" ref="Z226:Z230" si="37">X226+Y226</f>
+        <f t="shared" ref="Z226:Z230" si="57">X226+Y226</f>
         <v>17839.925999999999</v>
       </c>
     </row>
@@ -23233,11 +23227,11 @@
         <v>0.2</v>
       </c>
       <c r="O227" s="7">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="P227" s="7">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="Q227" s="11">
@@ -23251,27 +23245,27 @@
         <v>0.25</v>
       </c>
       <c r="U227" s="7">
-        <f>L227-(V227+W227+X227+Y227)</f>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="V227" s="7">
-        <f>Q227*L227</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="W227" s="7">
-        <f>R227*P227</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X227" s="7">
-        <f>S227*O227</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="Y227" s="7">
-        <f>T227*P227</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Z227" s="61">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
     </row>
@@ -23315,11 +23309,11 @@
         <v>0.1</v>
       </c>
       <c r="O228" s="7">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="P228" s="7">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="Q228" s="11">
@@ -23333,27 +23327,27 @@
         <v>0.25</v>
       </c>
       <c r="U228" s="7">
-        <f>L228-(V228+W228+X228+Y228)</f>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="V228" s="7">
-        <f>Q228*L228</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="W228" s="7">
-        <f>R228*P228</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X228" s="7">
-        <f>S228*O228</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="Y228" s="7">
-        <f>T228*P228</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Z228" s="17">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
     </row>
@@ -23399,11 +23393,11 @@
         <v>0.2</v>
       </c>
       <c r="O229" s="7">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>210232.12000000002</v>
       </c>
       <c r="P229" s="7">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>52558.030000000006</v>
       </c>
       <c r="Q229" s="11">
@@ -23417,27 +23411,27 @@
         <v>0.18</v>
       </c>
       <c r="U229" s="7">
-        <f>L229-(V229+W229+X229+Y229)</f>
+        <f t="shared" si="50"/>
         <v>216539.08360000001</v>
       </c>
       <c r="V229" s="7">
-        <f>Q229*L229</f>
+        <f t="shared" si="53"/>
         <v>15767.409000000001</v>
       </c>
       <c r="W229" s="7">
-        <f>R229*P229</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X229" s="7">
-        <f>S229*O229</f>
+        <f t="shared" si="52"/>
         <v>21023.212000000003</v>
       </c>
       <c r="Y229" s="7">
-        <f>T229*P229</f>
+        <f t="shared" si="54"/>
         <v>9460.4454000000005</v>
       </c>
       <c r="Z229" s="17">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>30483.657400000004</v>
       </c>
     </row>
@@ -23483,11 +23477,11 @@
         <v>0.05</v>
       </c>
       <c r="O230" s="7">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>1145721.3369999998</v>
       </c>
       <c r="P230" s="7">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>60301.123</v>
       </c>
       <c r="Q230" s="11">
@@ -23501,27 +23495,27 @@
         <v>0.22</v>
       </c>
       <c r="U230" s="7">
-        <f>L230-(V230+W230+X230+Y230)</f>
+        <f t="shared" si="50"/>
         <v>937079.45142000006</v>
       </c>
       <c r="V230" s="7">
-        <f>Q230*L230</f>
+        <f t="shared" si="53"/>
         <v>72361.347599999994</v>
       </c>
       <c r="W230" s="7">
-        <f>R230*P230</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X230" s="17">
-        <f>S230*O230</f>
+        <f t="shared" si="52"/>
         <v>183315.41391999996</v>
       </c>
       <c r="Y230" s="7">
-        <f>T230*P230</f>
+        <f t="shared" si="54"/>
         <v>13266.24706</v>
       </c>
       <c r="Z230" s="17">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>196581.66097999996</v>
       </c>
     </row>
@@ -23535,20 +23529,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3bb9dc88-f2da-4766-8908-3ca1e2958d73" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3bb9dc88-f2da-4766-8908-3ca1e2958d73" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23758,14 +23752,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0263AF5-3235-4A9E-A81A-1A30FD513646}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC4B4EE4-57DD-4509-98F8-31AD878EA5A5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -23777,6 +23763,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0263AF5-3235-4A9E-A81A-1A30FD513646}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>